<commit_message>
Bug Fixing: hotwaterenergy calculation
hotwaterenergy = hotwaterdemand * (BuildingInstance.heating_energy / BuildingInstance.heating_demand)

Here the formerly division with the efficiency of the heat generation was replaced by the mulitplication. Than the example was recalculated.
</commit_message>
<xml_diff>
--- a/iso_simulator/annualSimulation/results/annualResults_summary.xlsx
+++ b/iso_simulator/annualSimulation/results/annualResults_summary.xlsx
@@ -888,16 +888,16 @@
         <v>7.099999999999999</v>
       </c>
       <c r="Y2">
-        <v>1461.421188596631</v>
+        <v>1545.169778625117</v>
       </c>
       <c r="Z2">
-        <v>6.906370690062943</v>
+        <v>7.302148999574287</v>
       </c>
       <c r="AA2">
-        <v>223.48849856383</v>
+        <v>243.5881601706667</v>
       </c>
       <c r="AB2">
-        <v>1.056159872383944</v>
+        <v>1.151146666666667</v>
       </c>
       <c r="AC2">
         <v>7647.08545014216</v>
@@ -1049,16 +1049,16 @@
         <v>17.3</v>
       </c>
       <c r="Y3">
-        <v>11923.66171365018</v>
+        <v>11959.50849732252</v>
       </c>
       <c r="Z3">
-        <v>17.27405994467361</v>
+        <v>17.32599193543705</v>
       </c>
       <c r="AA3">
-        <v>1611.493771483711</v>
+        <v>1617.946192544732</v>
       </c>
       <c r="AB3">
-        <v>2.334604979375589</v>
+        <v>2.343952737713009</v>
       </c>
       <c r="AC3">
         <v>19846.29498696215</v>
@@ -1210,16 +1210,16 @@
         <v>10</v>
       </c>
       <c r="Y4">
-        <v>907.9388197600202</v>
+        <v>920.4965612866991</v>
       </c>
       <c r="Z4">
-        <v>9.932261566012095</v>
+        <v>10.06963511013957</v>
       </c>
       <c r="AA4">
-        <v>68.55628122834715</v>
+        <v>72.44918110161763</v>
       </c>
       <c r="AB4">
-        <v>0.7499612334375176</v>
+        <v>0.7925470321170338</v>
       </c>
       <c r="AC4">
         <v>56509.04430121201</v>
@@ -1371,16 +1371,16 @@
         <v>79.00000000000001</v>
       </c>
       <c r="Y5">
-        <v>51566.26562839076</v>
+        <v>53473.9996952143</v>
       </c>
       <c r="Z5">
-        <v>77.58466229329122</v>
+        <v>80.45496716249664</v>
       </c>
       <c r="AA5">
-        <v>10414.86264995934</v>
+        <v>11006.26021067463</v>
       </c>
       <c r="AB5">
-        <v>15.66981032427583</v>
+        <v>16.55960483372951</v>
       </c>
       <c r="AC5">
         <v>48854.02451252063</v>
@@ -1532,16 +1532,16 @@
         <v>7.099999999999999</v>
       </c>
       <c r="Y6">
-        <v>4016.288786084757</v>
+        <v>4242.797033226667</v>
       </c>
       <c r="Z6">
-        <v>6.910262492093612</v>
+        <v>7.299983333333333</v>
       </c>
       <c r="AA6">
-        <v>490.1184618455267</v>
+        <v>544.4804411595852</v>
       </c>
       <c r="AB6">
-        <v>0.8432778129172815</v>
+        <v>0.9368108148148148</v>
       </c>
       <c r="AC6">
         <v>32742.40632574527</v>
@@ -1693,16 +1693,16 @@
         <v>10</v>
       </c>
       <c r="Y7">
-        <v>7188.373318591133</v>
+        <v>7206.456348488312</v>
       </c>
       <c r="Z7">
-        <v>9.987611057205051</v>
+        <v>10.01273583319321</v>
       </c>
       <c r="AA7">
-        <v>98.72040131243622</v>
+        <v>104.3261405805616</v>
       </c>
       <c r="AB7">
-        <v>0.1371632952297827</v>
+        <v>0.1449519757861107</v>
       </c>
       <c r="AC7">
         <v>291486.670089793</v>
@@ -1854,16 +1854,16 @@
         <v>24.19999999999999</v>
       </c>
       <c r="Y8">
-        <v>16228.21352035223</v>
+        <v>16632.26992707227</v>
       </c>
       <c r="Z8">
-        <v>23.90876237002467</v>
+        <v>24.50405208569424</v>
       </c>
       <c r="AA8">
-        <v>1078.250507169657</v>
+        <v>1175.224044782467</v>
       </c>
       <c r="AB8">
-        <v>1.588568890774514</v>
+        <v>1.731438422535211</v>
       </c>
       <c r="AC8">
         <v>73595.14859390126</v>
@@ -2015,16 +2015,16 @@
         <v>7.1</v>
       </c>
       <c r="Y9">
-        <v>1781.422978839199</v>
+        <v>1784.997211823123</v>
       </c>
       <c r="Z9">
-        <v>7.092891547683687</v>
+        <v>7.107122669220945</v>
       </c>
       <c r="AA9">
-        <v>160.6798044720903</v>
+        <v>161.3231664091966</v>
       </c>
       <c r="AB9">
-        <v>0.6397607084681212</v>
+        <v>0.6423223103448277</v>
       </c>
       <c r="AC9">
         <v>8670.875372291339</v>
@@ -2176,16 +2176,16 @@
         <v>8.1</v>
       </c>
       <c r="Y10">
-        <v>5125.955277463337</v>
+        <v>5335.778096408275</v>
       </c>
       <c r="Z10">
-        <v>7.940973047958778</v>
+        <v>8.266024137931034</v>
       </c>
       <c r="AA10">
-        <v>559.9256865636146</v>
+        <v>610.2831631103999</v>
       </c>
       <c r="AB10">
-        <v>0.8674197384066585</v>
+        <v>0.9454319999999998</v>
       </c>
       <c r="AC10">
         <v>46825.99199593535</v>

</xml_diff>